<commit_message>
Updated to Version 4
</commit_message>
<xml_diff>
--- a/Docs/Mahda Log File Definitions v3.xlsx
+++ b/Docs/Mahda Log File Definitions v3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mahda\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK\Mahda\MLFProtocol\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431FCAD3-FED4-4E73-A8BB-FEB2CCC0BE28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E123C5E-F214-40E1-BAA1-81F5B036D14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="730" xr2:uid="{95B67488-F722-4AC5-8B20-B0817FF9564B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="730" activeTab="2" xr2:uid="{95B67488-F722-4AC5-8B20-B0817FF9564B}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="11" r:id="rId1"/>
@@ -143,9 +143,6 @@
     <t>{'M','A','H','D','A','L','O','G','F','I','L','E'}</t>
   </si>
   <si>
-    <t>ELEMENT_DATETIME</t>
-  </si>
-  <si>
     <t>Added Element Data Type field for each channel, Added Flag Field for Header</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>The string of Channel Name is now as Null Terminated so the bytes for Channel Name Size are removed</t>
+  </si>
+  <si>
+    <t>ELEMENT_DATETIME (uint64_t)</t>
   </si>
 </sst>
 </file>
@@ -767,7 +767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C242F9F8-F981-424B-AC7C-AC573712ECE9}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -817,7 +817,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
@@ -834,7 +834,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
@@ -849,7 +849,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -958,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09D7EA82-7352-46EB-88AC-6924F7A6F2B0}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1013,7 +1013,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="8"/>
     </row>
@@ -1165,7 +1165,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C20" s="1">
         <v>12</v>
@@ -1176,7 +1176,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="9"/>
     </row>
@@ -1185,7 +1185,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="9"/>
     </row>
@@ -1208,13 +1208,13 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.2">
@@ -1249,7 +1249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A59DCA-7E6F-4D46-8104-1482D696E71F}">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="1048576" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I1048576" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>